<commit_message>
Update Bootstrap test data
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3BE5D8-92C0-443A-A452-77AF0C053EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9444071-A378-4C8A-B699-F0B3488D7A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="1905" windowWidth="21585" windowHeight="14940" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="3330" yWindow="2355" windowWidth="21585" windowHeight="14940" activeTab="1" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
+    <sheet name="VT-Auth-NoCF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="72">
   <si>
     <t>Result</t>
   </si>
@@ -232,22 +233,25 @@
     <t>1478 Jhatka Palace</t>
   </si>
   <si>
-    <t>21054</t>
-  </si>
-  <si>
     <t>550 Swan Lake</t>
   </si>
   <si>
-    <t>03106</t>
-  </si>
-  <si>
     <t>25987 Hill Top</t>
   </si>
   <si>
-    <t>21093</t>
-  </si>
-  <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Suite 500</t>
+  </si>
+  <si>
+    <t>CardNameV</t>
+  </si>
+  <si>
+    <t>TULSI RAMAN</t>
+  </si>
+  <si>
+    <t>JANAKI JAMES</t>
   </si>
 </sst>
 </file>
@@ -623,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B27BFE-C179-457F-B2B0-1744259BA9C2}">
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,10 +645,12 @@
     <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
     <col min="14" max="28" width="12.140625" style="1"/>
     <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="12.140625" style="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,10 +741,13 @@
       <c r="AD1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -764,6 +773,15 @@
       <c r="L2" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="R2" s="1" t="s">
         <v>36</v>
       </c>
@@ -803,10 +821,13 @@
       <c r="AD2" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -832,6 +853,15 @@
       <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="R3" s="1" t="s">
         <v>36</v>
       </c>
@@ -871,10 +901,13 @@
       <c r="AD3" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -900,6 +933,15 @@
       <c r="L4" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>36</v>
       </c>
@@ -939,10 +981,13 @@
       <c r="AD4" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -968,6 +1013,15 @@
       <c r="L5" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1007,10 +1061,13 @@
       <c r="AD5" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1039,6 +1096,9 @@
       <c r="M6" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="O6" s="1" t="s">
         <v>63</v>
       </c>
@@ -1081,10 +1141,13 @@
       <c r="AD6" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1113,8 +1176,11 @@
       <c r="M7" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="O7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>36</v>
@@ -1155,10 +1221,13 @@
       <c r="AD7" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1185,10 +1254,13 @@
         <v>35</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>36</v>
@@ -1229,10 +1301,13 @@
       <c r="AD8" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1259,10 +1334,13 @@
         <v>35</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>36</v>
@@ -1302,6 +1380,9 @@
       </c>
       <c r="AD9" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1309,4 +1390,769 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="28" width="12.140625" style="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tab for SaleVoidNoCF
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9444071-A378-4C8A-B699-F0B3488D7A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D23749D-23CE-4CC6-9804-3004786C8E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="2355" windowWidth="21585" windowHeight="14940" activeTab="1" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="825" yWindow="735" windowWidth="21585" windowHeight="14940" activeTab="2" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
     <sheet name="VT-Auth-NoCF" sheetId="2" r:id="rId2"/>
+    <sheet name="VT-SaleVoid-NoCF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="72">
   <si>
     <t>Result</t>
   </si>
@@ -630,6 +631,773 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="28" width="12.140625" style="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1386,18 +2154,16 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6327E26-4C79-4401-A8C5-21FF97F5A24E}">
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Test data for Sale Demo Test Case
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D23749D-23CE-4CC6-9804-3004786C8E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1346A5-FE27-4856-8B1F-C85932EE539D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="735" windowWidth="21585" windowHeight="14940" activeTab="2" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="2985" yWindow="615" windowWidth="21585" windowHeight="14940" activeTab="3" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
     <sheet name="VT-Auth-NoCF" sheetId="2" r:id="rId2"/>
     <sheet name="VT-SaleVoid-NoCF" sheetId="3" r:id="rId3"/>
+    <sheet name="VT-Sale-NoCF-Demo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="74">
   <si>
     <t>Result</t>
   </si>
@@ -253,6 +254,12 @@
   </si>
   <si>
     <t>JANAKI JAMES</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>Access Change Me</t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6327E26-4C79-4401-A8C5-21FF97F5A24E}">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2921,4 +2928,770 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0B3AF-1323-47BA-A321-CEBD9FBB27E2}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="28" width="12.140625" style="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Sale NoCF Generic Test Data
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1346A5-FE27-4856-8B1F-C85932EE539D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C18291-B1C7-4378-BECD-6056E92F930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="615" windowWidth="21585" windowHeight="14940" activeTab="3" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="2985" yWindow="615" windowWidth="21585" windowHeight="14940" firstSheet="3" activeTab="6" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
     <sheet name="VT-Auth-NoCF" sheetId="2" r:id="rId2"/>
     <sheet name="VT-SaleVoid-NoCF" sheetId="3" r:id="rId3"/>
-    <sheet name="VT-Sale-NoCF-Demo" sheetId="4" r:id="rId4"/>
+    <sheet name="VT-Sale-NoCF-QA" sheetId="6" r:id="rId4"/>
+    <sheet name="VT-Sale-NoCF-Demo" sheetId="4" r:id="rId5"/>
+    <sheet name="VT-Sale-NoCF-Prod" sheetId="5" r:id="rId6"/>
+    <sheet name="VT-Sale-NoCF-Generic" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="82">
   <si>
     <t>Result</t>
   </si>
@@ -256,10 +259,34 @@
     <t>JANAKI JAMES</t>
   </si>
   <si>
-    <t>1286</t>
-  </si>
-  <si>
-    <t>Access Change Me</t>
+    <t>a_Access AutoNoCFtpProd</t>
+  </si>
+  <si>
+    <t>4583</t>
+  </si>
+  <si>
+    <t>a_Access AutoNoCFtpDemo</t>
+  </si>
+  <si>
+    <t>4249</t>
+  </si>
+  <si>
+    <t>AppIDQA</t>
+  </si>
+  <si>
+    <t>AppNameQA</t>
+  </si>
+  <si>
+    <t>AppIDDemo</t>
+  </si>
+  <si>
+    <t>AppIDProd</t>
+  </si>
+  <si>
+    <t>AppNameDemo</t>
+  </si>
+  <si>
+    <t>AppNameProd</t>
   </si>
 </sst>
 </file>
@@ -2931,11 +2958,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0B3AF-1323-47BA-A321-CEBD9FBB27E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29E4099-67A8-4B75-B256-0F3E875A0236}">
   <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,10 +3082,10 @@
         <v>67</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>30</v>
@@ -3135,10 +3162,10 @@
         <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>30</v>
@@ -3215,10 +3242,10 @@
         <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>30</v>
@@ -3295,10 +3322,10 @@
         <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>30</v>
@@ -3375,10 +3402,10 @@
         <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>61</v>
@@ -3455,10 +3482,10 @@
         <v>67</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>61</v>
@@ -3535,10 +3562,10 @@
         <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>61</v>
@@ -3615,10 +3642,775 @@
         <v>67</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F0B3AF-1323-47BA-A321-CEBD9FBB27E2}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="28" width="12.140625" style="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>61</v>
@@ -3694,4 +4486,1665 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FEF63A-9B81-4958-ACAF-2A5DC6F5B6C0}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.140625" style="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" style="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="28" width="12.140625" style="1"/>
+    <col min="29" max="29" width="20.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="1"/>
+    <col min="31" max="31" width="24.7109375" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F87D544-043A-4E2A-88AC-E2072E1F830C}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test Date for Single and Dual CF Generic
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C18291-B1C7-4378-BECD-6056E92F930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF52DC34-2592-4760-8F9C-DB1A17C7D857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="615" windowWidth="21585" windowHeight="14940" firstSheet="3" activeTab="6" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="3075" yWindow="1635" windowWidth="21600" windowHeight="12735" firstSheet="5" activeTab="8" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="VT-Sale-NoCF-Demo" sheetId="4" r:id="rId5"/>
     <sheet name="VT-Sale-NoCF-Prod" sheetId="5" r:id="rId6"/>
     <sheet name="VT-Sale-NoCF-Generic" sheetId="9" r:id="rId7"/>
+    <sheet name="VT-Sale-SingleCF-Generic" sheetId="10" r:id="rId8"/>
+    <sheet name="VT-Sale-DualCF-Generic" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="94">
   <si>
     <t>Result</t>
   </si>
@@ -287,6 +289,42 @@
   </si>
   <si>
     <t>AppNameProd</t>
+  </si>
+  <si>
+    <t>743</t>
+  </si>
+  <si>
+    <t>a_Access AutoSingleCFtpQA</t>
+  </si>
+  <si>
+    <t>4250</t>
+  </si>
+  <si>
+    <t>a_Access AutoSingleCFtpDemo</t>
+  </si>
+  <si>
+    <t>4584</t>
+  </si>
+  <si>
+    <t>a_Access AutoSingleCFtpProd</t>
+  </si>
+  <si>
+    <t>744</t>
+  </si>
+  <si>
+    <t>a_Access AutoDualCFtpQA</t>
+  </si>
+  <si>
+    <t>4251</t>
+  </si>
+  <si>
+    <t>a_Access AutoDualCFtpDemo</t>
+  </si>
+  <si>
+    <t>4585</t>
+  </si>
+  <si>
+    <t>a_Access AutoDualCFtpProd</t>
   </si>
 </sst>
 </file>
@@ -5257,8 +5295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F87D544-043A-4E2A-88AC-E2072E1F830C}">
   <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,4 +6185,1796 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B968B157-8910-471B-87BA-7CC46E0AB45F}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69067CF8-28FC-4E68-B131-0C0578E97988}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data for Sale Credit
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E5498E-4803-421C-9EEF-8FC9BA5E6115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529A57D-6E87-4B19-AB9D-BCFD01846CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="771" firstSheet="8" activeTab="14" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="31170" yWindow="1770" windowWidth="21600" windowHeight="12735" tabRatio="771" firstSheet="14" activeTab="16" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,9 @@
     <sheet name="VT-SaleVoid-NoCF-Generic" sheetId="15" r:id="rId13"/>
     <sheet name="VT-SaleVoid-SingleCF-Generic" sheetId="16" r:id="rId14"/>
     <sheet name="VT-SaleVoid-DualCF-Generic" sheetId="17" r:id="rId15"/>
+    <sheet name="VT-SaleCredit-NoCF-Generic" sheetId="18" r:id="rId16"/>
+    <sheet name="VT-SaleCredit-SingleCF-Generic" sheetId="19" r:id="rId17"/>
+    <sheet name="VT-SaleCredit-DualCF-Generic" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3909" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="99">
   <si>
     <t>Result</t>
   </si>
@@ -331,6 +334,21 @@
   </si>
   <si>
     <t>a_Access AutoDualCFtpProd</t>
+  </si>
+  <si>
+    <t>AutoCreditNumber</t>
+  </si>
+  <si>
+    <t>1200009876</t>
+  </si>
+  <si>
+    <t>4631220000</t>
+  </si>
+  <si>
+    <t>144963539</t>
+  </si>
+  <si>
+    <t>1100099302</t>
   </si>
 </sst>
 </file>
@@ -4164,7 +4182,7 @@
   <dimension ref="A1:AI9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5955,8 +5973,2724 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6204D91-76F9-4D6D-A5E4-EB5CFE343B83}">
   <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BF78E2-2FD7-4E12-B170-A75AAE6742DA}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03DBA54-ED01-4791-84D7-55AE2E626F53}">
+  <dimension ref="A1:AJ9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AI13" sqref="AI13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.5703125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB20E3F1-C4A0-4DB3-BD74-0C25E6E1CBA8}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Test data for Auth and Capture
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7529A57D-6E87-4B19-AB9D-BCFD01846CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEBEB08-62EA-4FF6-98CD-79ECD13774D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31170" yWindow="1770" windowWidth="21600" windowHeight="12735" tabRatio="771" firstSheet="14" activeTab="16" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="771" firstSheet="15" activeTab="20" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
     <sheet name="VT-SaleCredit-NoCF-Generic" sheetId="18" r:id="rId16"/>
     <sheet name="VT-SaleCredit-SingleCF-Generic" sheetId="19" r:id="rId17"/>
     <sheet name="VT-SaleCredit-DualCF-Generic" sheetId="20" r:id="rId18"/>
+    <sheet name="VT-AuthCapture-NoCF-Generic" sheetId="21" r:id="rId19"/>
+    <sheet name="VT-AuthCapture-SingleCF-Generic" sheetId="22" r:id="rId20"/>
+    <sheet name="VT-AuthCapture-DualCF-Generic" sheetId="23" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5613" uniqueCount="108">
   <si>
     <t>Result</t>
   </si>
@@ -349,6 +352,33 @@
   </si>
   <si>
     <t>1100099302</t>
+  </si>
+  <si>
+    <t>CaptureAmount</t>
+  </si>
+  <si>
+    <t>8.50</t>
+  </si>
+  <si>
+    <t>6.50</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>AmountwithCF</t>
+  </si>
+  <si>
+    <t>15.50</t>
+  </si>
+  <si>
+    <t>13.50</t>
+  </si>
+  <si>
+    <t>11.50</t>
+  </si>
+  <si>
+    <t>15.00</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1524,7 @@
   <dimension ref="A1:AI9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,7 +3316,7 @@
   <dimension ref="A1:AI9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7765,7 +7795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03DBA54-ED01-4791-84D7-55AE2E626F53}">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
@@ -9581,6 +9611,930 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E27B5D9-5032-44E3-84E3-DE165915798B}">
+  <dimension ref="A1:AJ9"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1:AJ9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1476F1-7EFE-4E48-BC46-8549E9104F90}">
   <dimension ref="A1:AE9"/>
@@ -10339,6 +11293,1910 @@
       </c>
       <c r="AE9" s="1" t="s">
         <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032979C1-8E13-45E8-AA46-AA2C52C9A8C1}">
+  <dimension ref="A1:AK9"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1:AK9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="18.7109375" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1337E-1CCF-48A2-B6FB-BAE32E7E4A51}">
+  <dimension ref="A1:AK9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" style="1" customWidth="1"/>
+    <col min="37" max="37" width="18.5703125" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test Data for Manual Auth
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEBEB08-62EA-4FF6-98CD-79ECD13774D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27577205-B28C-44A0-85EC-3A33555542F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="771" firstSheet="15" activeTab="20" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="31935" yWindow="1230" windowWidth="21600" windowHeight="12735" tabRatio="771" firstSheet="18" activeTab="21" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="VT-AuthCapture-NoCF-Generic" sheetId="21" r:id="rId19"/>
     <sheet name="VT-AuthCapture-SingleCF-Generic" sheetId="22" r:id="rId20"/>
     <sheet name="VT-AuthCapture-DualCF-Generic" sheetId="23" r:id="rId21"/>
+    <sheet name="VT-ManualAuthCapture-Generic" sheetId="24" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5613" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5835" uniqueCount="108">
   <si>
     <t>Result</t>
   </si>
@@ -12256,7 +12257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1337E-1CCF-48A2-B6FB-BAE32E7E4A51}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
@@ -13197,6 +13198,740 @@
       </c>
       <c r="AK9" s="1" t="s">
         <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17271EBE-670B-4D28-BBDF-B37E570C7236}">
+  <dimension ref="A1:AJ7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test date for Field Validation
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-Data.xlsx
+++ b/Bootstrap/VT-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27577205-B28C-44A0-85EC-3A33555542F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CE0309-0785-4318-8A1C-E319CFB505C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31935" yWindow="1230" windowWidth="21600" windowHeight="12735" tabRatio="771" firstSheet="18" activeTab="21" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
+    <workbookView xWindow="5145" yWindow="2385" windowWidth="21600" windowHeight="12735" tabRatio="771" firstSheet="20" activeTab="23" xr2:uid="{F6D5B6E5-5530-44B1-A3FD-270D512FE765}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-Sale-NoCF" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,8 @@
     <sheet name="VT-AuthCapture-SingleCF-Generic" sheetId="22" r:id="rId20"/>
     <sheet name="VT-AuthCapture-DualCF-Generic" sheetId="23" r:id="rId21"/>
     <sheet name="VT-ManualAuthCapture-Generic" sheetId="24" r:id="rId22"/>
+    <sheet name="VT-AuthCapVoid-Generic" sheetId="25" r:id="rId23"/>
+    <sheet name="VT-AuthCapCredit-Generic" sheetId="26" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5835" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6217" uniqueCount="108">
   <si>
     <t>Result</t>
   </si>
@@ -13209,8 +13211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17271EBE-670B-4D28-BBDF-B37E570C7236}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13931,6 +13933,1284 @@
         <v>71</v>
       </c>
       <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AD5C19-1571-4D0A-A553-7E96DEC1AB05}">
+  <dimension ref="A1:AJ7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9831DEED-0542-40B2-842B-1196FAE6B383}">
+  <dimension ref="A1:AJ5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="12.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>